<commit_message>
Fix bug of tassel test inside the container and add instruction of docker hub in readme
</commit_message>
<xml_diff>
--- a/sample_test/Tassel_test/trait.xlsx
+++ b/sample_test/Tassel_test/trait.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="trait_pixel" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="trait_cm" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="trait_pixel" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="trait_cm" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -440,32 +440,32 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>tassel_area_ratio</t>
+          <t>tassel_area ratio</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>avg_width</t>
+          <t>average_width</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>avg_height</t>
+          <t>average_height</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>number of branches</t>
+          <t>number_branches</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>avg branch length</t>
+          <t>average_branch_length</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>coins_width_avg</t>
+          <t>average_coins_width</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -475,7 +475,7 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>pixel_cm_ratio</t>
+          <t>pixel/cm_ratio</t>
         </is>
       </c>
     </row>
@@ -503,19 +503,19 @@
         <v>2037</v>
       </c>
       <c r="G2" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H2" t="n">
-        <v>382</v>
+        <v>587</v>
       </c>
       <c r="I2" t="n">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J2" t="n">
         <v>2.7</v>
       </c>
       <c r="K2" t="n">
-        <v>44.07407407407407</v>
+        <v>43.7037037037037</v>
       </c>
     </row>
   </sheetData>
@@ -560,27 +560,27 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>avg_width</t>
+          <t>average_width</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>avg_height</t>
+          <t>average_height</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>number of branches</t>
+          <t>number_of_branches</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>avg branch length</t>
+          <t>average_branch_length</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>coins_width_avg</t>
+          <t>average_coins_width</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
@@ -590,7 +590,7 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>pixel_cm_ratio</t>
+          <t>pixel/cm_ratio</t>
         </is>
       </c>
     </row>
@@ -606,22 +606,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>123.0705511616411</v>
+        <v>125.1653314421143</v>
       </c>
       <c r="D2" t="n">
         <v>0.1561825774935201</v>
       </c>
       <c r="E2" t="n">
-        <v>30.1764705882353</v>
+        <v>30.43220338983051</v>
       </c>
       <c r="F2" t="n">
-        <v>46.21764705882354</v>
+        <v>46.60932203389831</v>
       </c>
       <c r="G2" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H2" t="n">
-        <v>8.667226890756304</v>
+        <v>13.43135593220339</v>
       </c>
       <c r="I2" t="n">
         <v>2.7</v>
@@ -630,7 +630,7 @@
         <v>2.7</v>
       </c>
       <c r="K2" t="n">
-        <v>44.07407407407407</v>
+        <v>43.7037037037037</v>
       </c>
     </row>
   </sheetData>

</xml_diff>